<commit_message>
cambios antes de cambios del server
</commit_message>
<xml_diff>
--- a/public/build/files/invitados.xlsx
+++ b/public/build/files/invitados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto Santizo\Desktop\PROYECTOS\Boda Hermano Willy\Boda\public\build\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC148AA-0539-497D-AD38-48D2453D2302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA95A8CB-D99C-435A-B3DB-8681182070EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>